<commit_message>
Added final code and a PDF of my presentation slides
</commit_message>
<xml_diff>
--- a/ML test results 2.xlsx
+++ b/ML test results 2.xlsx
@@ -292,12 +292,6 @@
     <t>SVC(C=10, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma=10, kernel='rbf', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False), log transform</t>
   </si>
   <si>
-    <t>SVC(C=10, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma=1, kernel='rbf', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False), log transform</t>
-  </si>
-  <si>
-    <t>SVC(C=100, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma=1, kernel='rbf', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False), log transform</t>
-  </si>
-  <si>
     <t>SVC(C=10, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma=10, kernel='rbf', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False)
 NO PCA, log transform</t>
   </si>
@@ -340,6 +334,12 @@
       </rPr>
       <t>, average=False, class_weight=None, early_stopping=False, epsilon=0.1, eta0=0.0, fit_intercept=True, l1_ratio=0.15, learning_rate='optimal', loss='hinge', max_iter=1000, n_iter_no_change=5, n_jobs=None, penalty='none', power_t=0.5, random_state=None, shuffle=True, tol=0.001, validation_fraction=0.1, verbose=0, warm_start=False)</t>
     </r>
+  </si>
+  <si>
+    <t>SVC(C=10, cache_size=200, class_weight=None, coef0=0.0, decision_function_shapace='ovr', degree=3, gamma=1, kernel='rbf', max_iter=-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False), log transform</t>
+  </si>
+  <si>
+    <t>SVC(C=100, cache_size=200, class_weight=None, coef0=0.0, decision_function_shape='ovr', degree=3, gamma=1, kernel='rbf', A1:G26-1, probability=False, random_state=None, shrinking=True, tol=0.001, verbose=False), log transform</t>
   </si>
 </sst>
 </file>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="136" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1">
         <v>52</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1">
         <v>73.03</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1">
         <v>97.74</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1">
         <v>76.400000000000006</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1">
         <v>95.59</v>
@@ -1290,7 +1290,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1">
         <v>20.38</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1">
         <v>43.9</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1">
         <v>0.87</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33">
         <v>0.95</v>
@@ -1719,7 +1719,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>